<commit_message>
Replace HedStringDelimiter with HedString, intended to be used more places. Update json and definition handling to support placeholders more fully Handle definitions in json files better, improve errors for definitions. Remove Tilde support, add error for invalid tilde chars. Issue errors on poorly formatted tags, rather than automatically fixing them
</commit_message>
<xml_diff>
--- a/hedtools/examples/data/hed3_tags_single_sheet.xlsx
+++ b/hedtools/examples/data/hed3_tags_single_sheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t xml:space="preserve">Event code</t>
   </si>
@@ -40,22 +40,25 @@
     <t xml:space="preserve">Vehicle undergoes a perturbation to left.</t>
   </si>
   <si>
+    <t xml:space="preserve">Attribute/Sensory/Bisual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PerturbRight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vehicle undergoes a perturbation to right.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensory event, (Awake ~ Age/15 ~ Siren, Vehicle, RGB Red/100)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResponseOnset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subject starts to respond to perturbation by steering vehicle back to center of the lane.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Event/Sensory event, (Participant/Cognitive state/Awake ~ Participant/Trait/Age/15 ~ Item/Sound/Siren, Item/Object/Manmade/Vehicle, Attribute/Sensory/Visual/Color/RGB color/RGB Red/100)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PerturbRight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vehicle undergoes a perturbation to right.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sensory event, (Awake ~ Age/15 ~ Siren, Vehicle, RGB Red/100)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ResponseOnset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subject starts to respond to perturbation by steering vehicle back to center of the lane.</t>
   </si>
   <si>
     <t xml:space="preserve">ResponseOffset</t>
@@ -71,7 +74,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -101,12 +104,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -172,7 +169,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -196,7 +193,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -222,7 +219,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>251</v>
       </c>
@@ -261,7 +258,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -269,13 +266,13 @@
         <v>254</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update HedString further, use in more places.  Update validation to only work on long tags.  Misc other cleanup and fixes
</commit_message>
<xml_diff>
--- a/hedtools/examples/data/hed3_tags_single_sheet.xlsx
+++ b/hedtools/examples/data/hed3_tags_single_sheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Event code</t>
   </si>
@@ -40,7 +40,7 @@
     <t xml:space="preserve">Vehicle undergoes a perturbation to left.</t>
   </si>
   <si>
-    <t xml:space="preserve">Attribute/Sensory/Bisual</t>
+    <t xml:space="preserve">Attribute/Sensory/Visual</t>
   </si>
   <si>
     <t xml:space="preserve">PerturbRight</t>
@@ -49,22 +49,7 @@
     <t xml:space="preserve">Vehicle undergoes a perturbation to right.</t>
   </si>
   <si>
-    <t xml:space="preserve">Sensory event, (Awake ~ Age/15 ~ Siren, Vehicle, RGB Red/100)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ResponseOnset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subject starts to respond to perturbation by steering vehicle back to center of the lane.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Event/Sensory event, (Participant/Cognitive state/Awake ~ Participant/Trait/Age/15 ~ Item/Sound/Siren, Item/Object/Manmade/Vehicle, Attribute/Sensory/Visual/Color/RGB color/RGB Red/100)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ResponseOffset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subject completes response to perturbation having steered the vehicle back to the center of the lane.</t>
+    <t xml:space="preserve">Awake</t>
   </si>
 </sst>
 </file>
@@ -192,8 +177,8 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -233,7 +218,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>252</v>
       </c>
@@ -247,34 +232,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>253</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>254</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
+    <row r="4" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>